<commit_message>
Exploración de datos sobre el clima
</commit_message>
<xml_diff>
--- a/data/raw/estadisticas_normales_9120/Estadísticas normales Datos abiertos 1991-2020.xlsx
+++ b/data/raw/estadisticas_normales_9120/Estadísticas normales Datos abiertos 1991-2020.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Datos en la WEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbustos_lightech\Documents\Python Scripts\Contar con datos\dengue_y_zika\data\raw\estadisticas_normales_9120\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4581B8E3-279B-4135-A6C4-F2B8D0343DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estadísticas normales Datos abi" sheetId="1" r:id="rId1"/>
@@ -395,7 +396,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -890,9 +891,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -903,50 +901,53 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1223,14 +1224,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N789"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
@@ -1238,98 +1239,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>